<commit_message>
implementando el metodo de buscar producto por codigo
</commit_message>
<xml_diff>
--- a/target/classes/control/ventas/backend/excel/productos.xlsx
+++ b/target/classes/control/ventas/backend/excel/productos.xlsx
@@ -178,18 +178,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -200,6 +188,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -509,190 +509,190 @@
   <dimension ref="B2:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="L10" sqref="L10:M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="9" t="s">
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9" t="s">
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9" t="s">
+      <c r="K7" s="5"/>
+      <c r="L7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M7" s="9"/>
+      <c r="M7" s="5"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="4" t="s">
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="4">
+      <c r="H8" s="8"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="10">
         <v>260</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="4">
+      <c r="K8" s="9"/>
+      <c r="L8" s="10">
         <v>15</v>
       </c>
-      <c r="M8" s="5"/>
+      <c r="M8" s="9"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="4" t="s">
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="4">
+      <c r="H9" s="8"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="10">
         <v>250</v>
       </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="4">
+      <c r="K9" s="9"/>
+      <c r="L9" s="10">
         <v>12</v>
       </c>
-      <c r="M9" s="5"/>
+      <c r="M9" s="9"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="4" t="s">
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="4">
+      <c r="H10" s="8"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="10">
         <v>150</v>
       </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="4">
+      <c r="K10" s="9"/>
+      <c r="L10" s="10">
         <v>11</v>
       </c>
-      <c r="M10" s="5"/>
+      <c r="M10" s="9"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="7" t="s">
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7">
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11">
         <v>150</v>
       </c>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7">
-        <v>5</v>
-      </c>
-      <c r="M11" s="7"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11">
+        <v>10</v>
+      </c>
+      <c r="M11" s="11"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
@@ -920,28 +920,28 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="G8:I8"/>
     <mergeCell ref="B2:M3"/>
     <mergeCell ref="B4:M5"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:M11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>